<commit_message>
update plate informaiton template
</commit_message>
<xml_diff>
--- a/templates/growth_plate_reader/DATE_plate_layout.xlsx
+++ b/templates/growth_plate_reader/DATE_plate_layout.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="strains" sheetId="1" r:id="rId1"/>
+    <sheet name="strain" sheetId="1" r:id="rId1"/>
     <sheet name="well" sheetId="5" r:id="rId2"/>
     <sheet name="media" sheetId="2" r:id="rId3"/>
-    <sheet name="selection" sheetId="3" r:id="rId4"/>
-    <sheet name="misc" sheetId="4" r:id="rId5"/>
+    <sheet name="pos_selection" sheetId="3" r:id="rId4"/>
+    <sheet name="neg_selection" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -31,22 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="65">
-  <si>
-    <t>op_rep_vol</t>
-  </si>
-  <si>
-    <t>blank</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>5ugmL_chlor</t>
-  </si>
-  <si>
-    <t>M9_glucose</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="99">
   <si>
     <t>B10</t>
   </si>
@@ -226,6 +211,123 @@
   </si>
   <si>
     <t>G09</t>
+  </si>
+  <si>
+    <t>A01</t>
+  </si>
+  <si>
+    <t>A02</t>
+  </si>
+  <si>
+    <t>A03</t>
+  </si>
+  <si>
+    <t>A04</t>
+  </si>
+  <si>
+    <t>A05</t>
+  </si>
+  <si>
+    <t>A06</t>
+  </si>
+  <si>
+    <t>A07</t>
+  </si>
+  <si>
+    <t>A08</t>
+  </si>
+  <si>
+    <t>A09</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>A11</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>B01</t>
+  </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>D01</t>
+  </si>
+  <si>
+    <t>E01</t>
+  </si>
+  <si>
+    <t>F01</t>
+  </si>
+  <si>
+    <t>G01</t>
+  </si>
+  <si>
+    <t>H01</t>
+  </si>
+  <si>
+    <t>B12</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>D12</t>
+  </si>
+  <si>
+    <t>E12</t>
+  </si>
+  <si>
+    <t>F12</t>
+  </si>
+  <si>
+    <t>G12</t>
+  </si>
+  <si>
+    <t>H02</t>
+  </si>
+  <si>
+    <t>H03</t>
+  </si>
+  <si>
+    <t>H04</t>
+  </si>
+  <si>
+    <t>H05</t>
+  </si>
+  <si>
+    <t>H06</t>
+  </si>
+  <si>
+    <t>H07</t>
+  </si>
+  <si>
+    <t>H08</t>
+  </si>
+  <si>
+    <t>H09</t>
+  </si>
+  <si>
+    <t>H10</t>
+  </si>
+  <si>
+    <t>H11</t>
+  </si>
+  <si>
+    <t>H12</t>
+  </si>
+  <si>
+    <t>M9_0.5%_glucose</t>
+  </si>
+  <si>
+    <t>x_units_compound</t>
+  </si>
+  <si>
+    <t>op_rep_selection</t>
   </si>
 </sst>
 </file>
@@ -540,204 +642,316 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="E1" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="F1" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="G1" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="H1" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="I1" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="J1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="K1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="D2" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="E2" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="F2" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="G2" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="H2" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="I2" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="J2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="K2" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="D3" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="E3" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="F3" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="G3" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="H3" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="I3" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="J3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="K3" t="s">
+        <v>98</v>
+      </c>
+      <c r="L3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="D4" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="E4" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="F4" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="G4" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="H4" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="I4" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="J4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="K4" t="s">
+        <v>98</v>
+      </c>
+      <c r="L4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="C5" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="D5" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="E5" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="F5" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="G5" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="H5" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="I5" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="J5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="K5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="C6" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="D6" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="E6" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="F6" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="G6" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="H6" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="I6" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="J6" t="s">
-        <v>1</v>
+        <v>98</v>
+      </c>
+      <c r="K6" t="s">
+        <v>98</v>
+      </c>
+      <c r="L6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G7" t="s">
+        <v>98</v>
+      </c>
+      <c r="H7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I7" t="s">
+        <v>98</v>
+      </c>
+      <c r="J7" t="s">
+        <v>98</v>
+      </c>
+      <c r="K7" t="s">
+        <v>98</v>
+      </c>
+      <c r="L7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" t="s">
+        <v>98</v>
+      </c>
+      <c r="H8" t="s">
+        <v>98</v>
+      </c>
+      <c r="I8" t="s">
+        <v>98</v>
+      </c>
+      <c r="J8" t="s">
+        <v>98</v>
+      </c>
+      <c r="K8" t="s">
+        <v>98</v>
+      </c>
+      <c r="L8" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -747,204 +961,316 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="H2" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
+      <c r="I2" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="J2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C3" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
+      <c r="D3" t="s">
         <v>22</v>
       </c>
-      <c r="G1" t="s">
+      <c r="E3" t="s">
         <v>23</v>
       </c>
-      <c r="H1" t="s">
+      <c r="F3" t="s">
         <v>24</v>
       </c>
-      <c r="I1" t="s">
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="K5" t="s">
         <v>7</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="K6" t="s">
         <v>9</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" t="s">
+        <v>59</v>
+      </c>
+      <c r="J7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="K7" t="s">
         <v>11</v>
       </c>
-      <c r="J4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" t="s">
-        <v>56</v>
-      </c>
-      <c r="I5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G6" t="s">
-        <v>63</v>
-      </c>
-      <c r="H6" t="s">
-        <v>64</v>
-      </c>
-      <c r="I6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" t="s">
-        <v>16</v>
+      <c r="L7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" t="s">
+        <v>89</v>
+      </c>
+      <c r="G8" t="s">
+        <v>90</v>
+      </c>
+      <c r="H8" t="s">
+        <v>91</v>
+      </c>
+      <c r="I8" t="s">
+        <v>92</v>
+      </c>
+      <c r="J8" t="s">
+        <v>93</v>
+      </c>
+      <c r="K8" t="s">
+        <v>94</v>
+      </c>
+      <c r="L8" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -954,10 +1280,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -965,196 +1291,308 @@
     <col min="1" max="1" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="G1" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="H1" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="I1" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="J1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="F2" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="G2" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="H2" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="I2" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="J2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="E3" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="F3" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="G3" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="H3" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="I3" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="J3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K3" t="s">
+        <v>96</v>
+      </c>
+      <c r="L3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="E4" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="F4" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="G4" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="H4" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="I4" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="J4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K4" t="s">
+        <v>96</v>
+      </c>
+      <c r="L4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="F5" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="G5" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="H5" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="I5" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="J5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="D6" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="E6" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="F6" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="G6" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="H6" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="I6" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="J6" t="s">
-        <v>4</v>
+        <v>96</v>
+      </c>
+      <c r="K6" t="s">
+        <v>96</v>
+      </c>
+      <c r="L6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G7" t="s">
+        <v>96</v>
+      </c>
+      <c r="H7" t="s">
+        <v>96</v>
+      </c>
+      <c r="I7" t="s">
+        <v>96</v>
+      </c>
+      <c r="J7" t="s">
+        <v>96</v>
+      </c>
+      <c r="K7" t="s">
+        <v>96</v>
+      </c>
+      <c r="L7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G8" t="s">
+        <v>96</v>
+      </c>
+      <c r="H8" t="s">
+        <v>96</v>
+      </c>
+      <c r="I8" t="s">
+        <v>96</v>
+      </c>
+      <c r="J8" t="s">
+        <v>96</v>
+      </c>
+      <c r="K8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L8" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1164,204 +1602,319 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection sqref="A1:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="10" max="10" width="19.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="F1" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="G1" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="H1" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="I1" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="J1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="K1" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="F2" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="G2" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="H2" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="J2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="K2" t="s">
+        <v>97</v>
+      </c>
+      <c r="L2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="E3" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="F3" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="G3" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="H3" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="I3" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="J3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="K3" t="s">
+        <v>97</v>
+      </c>
+      <c r="L3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="E4" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="F4" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="G4" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="H4" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="I4" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="J4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="K4" t="s">
+        <v>97</v>
+      </c>
+      <c r="L4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="E5" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="F5" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="G5" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="H5" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="I5" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="J5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="K5" t="s">
+        <v>97</v>
+      </c>
+      <c r="L5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="E6" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="F6" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="G6" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="H6" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="I6" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="J6" t="s">
-        <v>3</v>
+        <v>97</v>
+      </c>
+      <c r="K6" t="s">
+        <v>97</v>
+      </c>
+      <c r="L6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H7" t="s">
+        <v>97</v>
+      </c>
+      <c r="I7" t="s">
+        <v>97</v>
+      </c>
+      <c r="J7" t="s">
+        <v>97</v>
+      </c>
+      <c r="K7" t="s">
+        <v>97</v>
+      </c>
+      <c r="L7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" t="s">
+        <v>97</v>
+      </c>
+      <c r="G8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" t="s">
+        <v>97</v>
+      </c>
+      <c r="I8" t="s">
+        <v>97</v>
+      </c>
+      <c r="J8" t="s">
+        <v>97</v>
+      </c>
+      <c r="K8" t="s">
+        <v>97</v>
+      </c>
+      <c r="L8" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1371,204 +1924,316 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection sqref="A1:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="F1" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="G1" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="H1" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="I1" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="J1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="K1" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="F2" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="G2" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="H2" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="J2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="K2" t="s">
+        <v>97</v>
+      </c>
+      <c r="L2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="E3" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="F3" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="G3" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="H3" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="I3" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="J3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="K3" t="s">
+        <v>97</v>
+      </c>
+      <c r="L3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="E4" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="F4" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="G4" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="H4" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="I4" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="J4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="K4" t="s">
+        <v>97</v>
+      </c>
+      <c r="L4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="E5" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="F5" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="G5" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="H5" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="I5" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="J5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="K5" t="s">
+        <v>97</v>
+      </c>
+      <c r="L5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="E6" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="F6" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="G6" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="H6" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="I6" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="J6" t="s">
-        <v>2</v>
+        <v>97</v>
+      </c>
+      <c r="K6" t="s">
+        <v>97</v>
+      </c>
+      <c r="L6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H7" t="s">
+        <v>97</v>
+      </c>
+      <c r="I7" t="s">
+        <v>97</v>
+      </c>
+      <c r="J7" t="s">
+        <v>97</v>
+      </c>
+      <c r="K7" t="s">
+        <v>97</v>
+      </c>
+      <c r="L7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" t="s">
+        <v>97</v>
+      </c>
+      <c r="G8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" t="s">
+        <v>97</v>
+      </c>
+      <c r="I8" t="s">
+        <v>97</v>
+      </c>
+      <c r="J8" t="s">
+        <v>97</v>
+      </c>
+      <c r="K8" t="s">
+        <v>97</v>
+      </c>
+      <c r="L8" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added plate layout and information for 2020-03-03 experiment
</commit_message>
<xml_diff>
--- a/templates/growth_plate_reader/DATE_plate_layout.xlsx
+++ b/templates/growth_plate_reader/DATE_plate_layout.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/razo/Documents/PhD/evo_mwc/templates/growth_plate_reader/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gchure/Dropbox/git/mwc_evo/templates/growth_plate_reader/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D617E8-62FB-9046-AF78-D04C2D4B2585}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38300" windowHeight="23620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="strain" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <sheet name="pos_selection" sheetId="3" r:id="rId4"/>
     <sheet name="neg_selection" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="154">
   <si>
     <t>B10</t>
   </si>
@@ -327,17 +328,188 @@
     <t>x_units_compound</t>
   </si>
   <si>
-    <t>op_rep_selection</t>
+    <t>none_HG105_0.1</t>
+  </si>
+  <si>
+    <t>none_HG105_0.2</t>
+  </si>
+  <si>
+    <t>none_HG105_0.3</t>
+  </si>
+  <si>
+    <t>none_HG105_0.4</t>
+  </si>
+  <si>
+    <t>none_HG105_0.5</t>
+  </si>
+  <si>
+    <t>none_HG105_0.6</t>
+  </si>
+  <si>
+    <t>none_HG105_0.7</t>
+  </si>
+  <si>
+    <t>none_HG105_0.8</t>
+  </si>
+  <si>
+    <t>none_HG105_0.9</t>
+  </si>
+  <si>
+    <t>none_HG105_1.0</t>
+  </si>
+  <si>
+    <t>O2_R1740_0.0</t>
+  </si>
+  <si>
+    <t>none_HG105_0.0</t>
+  </si>
+  <si>
+    <t>O2_R1740_0.1</t>
+  </si>
+  <si>
+    <t>O2_R1740_0.2</t>
+  </si>
+  <si>
+    <t>O2_R1740_0.3</t>
+  </si>
+  <si>
+    <t>O2_R1740_0.4</t>
+  </si>
+  <si>
+    <t>O2_R1740_0.5</t>
+  </si>
+  <si>
+    <t>O2_R1740_0.6</t>
+  </si>
+  <si>
+    <t>O2_R1740_0.7</t>
+  </si>
+  <si>
+    <t>O2_R1740_0.8</t>
+  </si>
+  <si>
+    <t>O2_R1740_0.9</t>
+  </si>
+  <si>
+    <t>O2_R260_0.0</t>
+  </si>
+  <si>
+    <t>O2_R260_0.1</t>
+  </si>
+  <si>
+    <t>O2_R260_0.2</t>
+  </si>
+  <si>
+    <t>O2_R260_0.3</t>
+  </si>
+  <si>
+    <t>O2_R260_0.4</t>
+  </si>
+  <si>
+    <t>O2_R260_0.5</t>
+  </si>
+  <si>
+    <t>O2_R260_0.6</t>
+  </si>
+  <si>
+    <t>O2_R260_0.7</t>
+  </si>
+  <si>
+    <t>O2_R260_0.8</t>
+  </si>
+  <si>
+    <t>O2_R260_0.9</t>
+  </si>
+  <si>
+    <t>O2_R22_0.0</t>
+  </si>
+  <si>
+    <t>O2_R22_0.1</t>
+  </si>
+  <si>
+    <t>O2_R22_0.2</t>
+  </si>
+  <si>
+    <t>O2_R22_0.3</t>
+  </si>
+  <si>
+    <t>O2_R22_0.4</t>
+  </si>
+  <si>
+    <t>O2_R22_0.5</t>
+  </si>
+  <si>
+    <t>O2_R22_0.6</t>
+  </si>
+  <si>
+    <t>O2_R22_0.7</t>
+  </si>
+  <si>
+    <t>O2_R22_0.8</t>
+  </si>
+  <si>
+    <t>O2_R22_0.9</t>
+  </si>
+  <si>
+    <t>O2_R1740_1.0</t>
+  </si>
+  <si>
+    <t>O2_R260_1.0</t>
+  </si>
+  <si>
+    <t>O2_R22_1.0</t>
+  </si>
+  <si>
+    <t>O2_R0_0.0</t>
+  </si>
+  <si>
+    <t>O2_R0_0.1</t>
+  </si>
+  <si>
+    <t>O2_R0_0.2</t>
+  </si>
+  <si>
+    <t>O2_R0_0.3</t>
+  </si>
+  <si>
+    <t>O2_R0_0.4</t>
+  </si>
+  <si>
+    <t>O2_R0_0.5</t>
+  </si>
+  <si>
+    <t>O2_R0_0.6</t>
+  </si>
+  <si>
+    <t>O2_R0_0.7</t>
+  </si>
+  <si>
+    <t>O2_R0_0.8</t>
+  </si>
+  <si>
+    <t>O2_R0_0.9</t>
+  </si>
+  <si>
+    <t>O2_R0_1.0</t>
+  </si>
+  <si>
+    <t>blank</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -374,6 +546,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -641,326 +816,245 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="5" max="6" width="21.5" customWidth="1"/>
+    <col min="7" max="7" width="15.5" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1"/>
+    <col min="10" max="10" width="41.5" customWidth="1"/>
+    <col min="11" max="11" width="38.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="B1" t="s">
         <v>98</v>
       </c>
       <c r="C1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="G1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="H1" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="I1" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="J1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="K1" t="s">
-        <v>98</v>
-      </c>
-      <c r="L1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="E2" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="F2" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="G2" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="H2" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="I2" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="J2" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="K2" t="s">
-        <v>98</v>
-      </c>
-      <c r="L2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
-        <v>98</v>
+        <v>121</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="E3" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
       <c r="F3" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="G3" t="s">
-        <v>98</v>
+        <v>125</v>
       </c>
       <c r="H3" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="I3" t="s">
-        <v>98</v>
+        <v>127</v>
       </c>
       <c r="J3" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
       <c r="K3" t="s">
-        <v>98</v>
-      </c>
-      <c r="L3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>129</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>131</v>
       </c>
       <c r="D4" t="s">
-        <v>98</v>
+        <v>132</v>
       </c>
       <c r="E4" t="s">
-        <v>98</v>
+        <v>133</v>
       </c>
       <c r="F4" t="s">
-        <v>98</v>
+        <v>134</v>
       </c>
       <c r="G4" t="s">
-        <v>98</v>
+        <v>135</v>
       </c>
       <c r="H4" t="s">
-        <v>98</v>
+        <v>136</v>
       </c>
       <c r="I4" t="s">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="J4" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="K4" t="s">
-        <v>98</v>
-      </c>
-      <c r="L4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>142</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>143</v>
       </c>
       <c r="C5" t="s">
-        <v>98</v>
+        <v>144</v>
       </c>
       <c r="D5" t="s">
-        <v>98</v>
+        <v>145</v>
       </c>
       <c r="E5" t="s">
-        <v>98</v>
+        <v>146</v>
       </c>
       <c r="F5" t="s">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="G5" t="s">
-        <v>98</v>
+        <v>148</v>
       </c>
       <c r="H5" t="s">
-        <v>98</v>
+        <v>149</v>
       </c>
       <c r="I5" t="s">
-        <v>98</v>
+        <v>150</v>
       </c>
       <c r="J5" t="s">
-        <v>98</v>
+        <v>151</v>
       </c>
       <c r="K5" t="s">
-        <v>98</v>
-      </c>
-      <c r="L5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>153</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>153</v>
       </c>
       <c r="C6" t="s">
-        <v>98</v>
+        <v>153</v>
       </c>
       <c r="D6" t="s">
-        <v>98</v>
+        <v>153</v>
       </c>
       <c r="E6" t="s">
-        <v>98</v>
+        <v>153</v>
       </c>
       <c r="F6" t="s">
-        <v>98</v>
+        <v>153</v>
       </c>
       <c r="G6" t="s">
-        <v>98</v>
+        <v>153</v>
       </c>
       <c r="H6" t="s">
-        <v>98</v>
+        <v>153</v>
       </c>
       <c r="I6" t="s">
-        <v>98</v>
+        <v>153</v>
       </c>
       <c r="J6" t="s">
-        <v>98</v>
+        <v>153</v>
       </c>
       <c r="K6" t="s">
-        <v>98</v>
-      </c>
-      <c r="L6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E7" t="s">
-        <v>98</v>
-      </c>
-      <c r="F7" t="s">
-        <v>98</v>
-      </c>
-      <c r="G7" t="s">
-        <v>98</v>
-      </c>
-      <c r="H7" t="s">
-        <v>98</v>
-      </c>
-      <c r="I7" t="s">
-        <v>98</v>
-      </c>
-      <c r="J7" t="s">
-        <v>98</v>
-      </c>
-      <c r="K7" t="s">
-        <v>98</v>
-      </c>
-      <c r="L7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>98</v>
-      </c>
-      <c r="B8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C8" t="s">
-        <v>98</v>
-      </c>
-      <c r="D8" t="s">
-        <v>98</v>
-      </c>
-      <c r="E8" t="s">
-        <v>98</v>
-      </c>
-      <c r="F8" t="s">
-        <v>98</v>
-      </c>
-      <c r="G8" t="s">
-        <v>98</v>
-      </c>
-      <c r="H8" t="s">
-        <v>98</v>
-      </c>
-      <c r="I8" t="s">
-        <v>98</v>
-      </c>
-      <c r="J8" t="s">
-        <v>98</v>
-      </c>
-      <c r="K8" t="s">
-        <v>98</v>
-      </c>
-      <c r="L8" t="s">
-        <v>98</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1279,7 +1373,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1601,7 +1695,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1923,7 +2017,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>